<commit_message>
remove TUI, add OutOfBound constraint, Overlap constraint and add tests for them
</commit_message>
<xml_diff>
--- a/data/conslay/f1_hoisting_time_data.xlsx
+++ b/data/conslay/f1_hoisting_time_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daovudat/Desktop/Projects/matlab/moaha-place-OBL/moaha_place_obl_3cases/multiphase/static/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daovudat/Desktop/Projects/freelance/golang-moaha-construction/data/conslay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CF76E1-EF0B-2546-B628-9D00640DF1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A22F13-B182-B947-997D-EA301DC30D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{3F942686-A653-0144-BFE0-507A5CD4C194}"/>
+    <workbookView xWindow="9620" yWindow="1520" windowWidth="28800" windowHeight="15800" xr2:uid="{3F942686-A653-0144-BFE0-507A5CD4C194}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Steel components install point</t>
   </si>
   <si>
-    <t>Symbol</t>
-  </si>
-  <si>
     <t>X-coordinate</t>
   </si>
   <si>
@@ -98,13 +95,25 @@
   </si>
   <si>
     <t>External wall panels #8</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>TF8</t>
+  </si>
+  <si>
+    <t>TF9</t>
+  </si>
+  <si>
+    <t>TF10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +125,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -175,6 +190,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,7 +511,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B10" sqref="B10:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,23 +524,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" s="3">
         <v>59</v>
       </c>
@@ -535,9 +555,11 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C3" s="3">
         <v>85</v>
       </c>
@@ -550,9 +572,11 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="3">
         <v>85</v>
       </c>
@@ -565,9 +589,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C5" s="3">
         <v>59</v>
       </c>
@@ -580,9 +606,11 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" s="4">
         <v>59</v>
       </c>
@@ -595,9 +623,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C7" s="4">
         <v>85</v>
       </c>
@@ -610,9 +640,11 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" s="4">
         <v>85</v>
       </c>
@@ -625,9 +657,11 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C9" s="4">
         <v>59</v>
       </c>
@@ -640,9 +674,11 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="3">
         <v>59</v>
       </c>
@@ -655,9 +691,11 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C11" s="3">
         <v>85</v>
       </c>
@@ -670,9 +708,11 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C12" s="3">
         <v>98</v>
       </c>
@@ -685,9 +725,11 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C13" s="3">
         <v>98</v>
       </c>
@@ -700,9 +742,11 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C14" s="3">
         <v>85</v>
       </c>
@@ -715,9 +759,11 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C15" s="3">
         <v>59</v>
       </c>
@@ -730,9 +776,11 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C16" s="3">
         <v>46</v>
       </c>
@@ -745,9 +793,11 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C17" s="3">
         <v>46</v>
       </c>
@@ -759,6 +809,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>